<commit_message>
Add dia chi danh muc xe
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Gara/Template_DanhSachXe.xlsx
+++ b/banhang24/Template/ExportExcel/Gara/Template_DanhSachXe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Mẫu xe</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Mã chủ xe</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
   </si>
 </sst>
 </file>
@@ -455,11 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,21 +470,22 @@
     <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -499,8 +503,9 @@
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-    </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="13"/>
+    </row>
+    <row r="3" spans="1:16" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -514,40 +519,43 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -555,16 +563,17 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="11"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -572,16 +581,17 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -589,16 +599,17 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -606,16 +617,17 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -623,16 +635,17 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -640,16 +653,17 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -657,16 +671,17 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -674,16 +689,17 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -691,16 +707,17 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -708,16 +725,17 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -725,16 +743,17 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -742,16 +761,17 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -759,16 +779,17 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -776,16 +797,17 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -793,16 +815,17 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -810,16 +833,17 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -827,16 +851,17 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -844,16 +869,17 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -861,16 +887,17 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -878,16 +905,17 @@
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -895,16 +923,17 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -912,16 +941,17 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -929,16 +959,17 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -946,16 +977,17 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="12"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -963,16 +995,17 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="12"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -980,16 +1013,17 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="12"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -997,16 +1031,17 @@
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="12"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1014,16 +1049,17 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="12"/>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1031,16 +1067,17 @@
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="12"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1048,16 +1085,17 @@
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -1065,16 +1103,17 @@
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34" s="10"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -1082,16 +1121,17 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="12"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -1099,16 +1139,17 @@
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -1116,16 +1157,17 @@
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="12"/>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" s="10"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -1133,16 +1175,17 @@
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="12"/>
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -1150,16 +1193,17 @@
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="12"/>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -1167,16 +1211,17 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="12"/>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -1184,16 +1229,17 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="12"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1201,16 +1247,17 @@
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="12"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -1218,16 +1265,17 @@
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="12"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -1235,16 +1283,17 @@
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="12"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -1252,16 +1301,17 @@
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="12"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P45" s="10"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -1269,16 +1319,17 @@
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="12"/>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46" s="10"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -1286,16 +1337,17 @@
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="12"/>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P47" s="10"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -1303,16 +1355,17 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="12"/>
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -1320,16 +1373,17 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="12"/>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49" s="10"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -1337,16 +1391,17 @@
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="12"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50" s="10"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -1354,16 +1409,17 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="12"/>
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51" s="10"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -1371,16 +1427,17 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="12"/>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P52" s="10"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
@@ -1388,16 +1445,17 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="12"/>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53" s="10"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -1405,16 +1463,17 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="12"/>
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
       <c r="O54" s="10"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P54" s="10"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -1422,16 +1481,17 @@
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="12"/>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
       <c r="O55" s="10"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P55" s="10"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -1439,16 +1499,17 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="12"/>
       <c r="J56" s="10"/>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P56" s="10"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -1456,16 +1517,17 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="12"/>
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
       <c r="O57" s="10"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P57" s="10"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -1473,16 +1535,17 @@
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="12"/>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
       <c r="O58" s="10"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P58" s="10"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -1490,16 +1553,17 @@
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="12"/>
       <c r="J59" s="10"/>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
       <c r="O59" s="10"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P59" s="10"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -1507,16 +1571,17 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="12"/>
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
       <c r="O60" s="10"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P60" s="10"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -1524,16 +1589,17 @@
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="12"/>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
       <c r="M61" s="10"/>
       <c r="N61" s="10"/>
       <c r="O61" s="10"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P61" s="10"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -1541,16 +1607,17 @@
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="12"/>
       <c r="J62" s="10"/>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P62" s="10"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -1558,16 +1625,17 @@
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="12"/>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
       <c r="M63" s="10"/>
       <c r="N63" s="10"/>
       <c r="O63" s="10"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P63" s="10"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -1575,16 +1643,17 @@
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="12"/>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P64" s="10"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -1592,16 +1661,17 @@
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="12"/>
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P65" s="10"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -1609,16 +1679,17 @@
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="12"/>
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
       <c r="O66" s="10"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P66" s="10"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
@@ -1626,16 +1697,17 @@
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="12"/>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
       <c r="O67" s="10"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P67" s="10"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -1643,16 +1715,17 @@
       <c r="E68" s="10"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="12"/>
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
       <c r="M68" s="10"/>
       <c r="N68" s="10"/>
       <c r="O68" s="10"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P68" s="10"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
@@ -1660,16 +1733,17 @@
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
-      <c r="H69" s="12"/>
-      <c r="I69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="12"/>
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
       <c r="M69" s="10"/>
       <c r="N69" s="10"/>
       <c r="O69" s="10"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P69" s="10"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -1677,16 +1751,17 @@
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="12"/>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
       <c r="M70" s="10"/>
       <c r="N70" s="10"/>
       <c r="O70" s="10"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P70" s="10"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
@@ -1694,16 +1769,17 @@
       <c r="E71" s="10"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="12"/>
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
       <c r="L71" s="10"/>
       <c r="M71" s="10"/>
       <c r="N71" s="10"/>
       <c r="O71" s="10"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P71" s="10"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -1711,16 +1787,17 @@
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="12"/>
       <c r="J72" s="10"/>
       <c r="K72" s="10"/>
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P72" s="10"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -1728,16 +1805,17 @@
       <c r="E73" s="10"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="12"/>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
       <c r="L73" s="10"/>
       <c r="M73" s="10"/>
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P73" s="10"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -1745,16 +1823,17 @@
       <c r="E74" s="10"/>
       <c r="F74" s="10"/>
       <c r="G74" s="10"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="12"/>
       <c r="J74" s="10"/>
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
       <c r="M74" s="10"/>
       <c r="N74" s="10"/>
       <c r="O74" s="10"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P74" s="10"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -1762,16 +1841,17 @@
       <c r="E75" s="10"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="12"/>
       <c r="J75" s="10"/>
       <c r="K75" s="10"/>
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
       <c r="N75" s="10"/>
       <c r="O75" s="10"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P75" s="10"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -1779,16 +1859,17 @@
       <c r="E76" s="10"/>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="12"/>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
       <c r="L76" s="10"/>
       <c r="M76" s="10"/>
       <c r="N76" s="10"/>
       <c r="O76" s="10"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P76" s="10"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -1796,16 +1877,17 @@
       <c r="E77" s="10"/>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="12"/>
       <c r="J77" s="10"/>
       <c r="K77" s="10"/>
       <c r="L77" s="10"/>
       <c r="M77" s="10"/>
       <c r="N77" s="10"/>
       <c r="O77" s="10"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P77" s="10"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -1813,16 +1895,17 @@
       <c r="E78" s="10"/>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="12"/>
       <c r="J78" s="10"/>
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
       <c r="M78" s="10"/>
       <c r="N78" s="10"/>
       <c r="O78" s="10"/>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P78" s="10"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -1830,16 +1913,17 @@
       <c r="E79" s="10"/>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="12"/>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
       <c r="M79" s="10"/>
       <c r="N79" s="10"/>
       <c r="O79" s="10"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P79" s="10"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -1847,16 +1931,17 @@
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="12"/>
       <c r="J80" s="10"/>
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
       <c r="M80" s="10"/>
       <c r="N80" s="10"/>
       <c r="O80" s="10"/>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P80" s="10"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
@@ -1864,16 +1949,17 @@
       <c r="E81" s="10"/>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="12"/>
       <c r="J81" s="10"/>
       <c r="K81" s="10"/>
       <c r="L81" s="10"/>
       <c r="M81" s="10"/>
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P81" s="10"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -1881,16 +1967,17 @@
       <c r="E82" s="10"/>
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="12"/>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
       <c r="M82" s="10"/>
       <c r="N82" s="10"/>
       <c r="O82" s="10"/>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P82" s="10"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -1898,16 +1985,17 @@
       <c r="E83" s="10"/>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="12"/>
       <c r="J83" s="10"/>
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
       <c r="M83" s="10"/>
       <c r="N83" s="10"/>
       <c r="O83" s="10"/>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P83" s="10"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -1915,16 +2003,17 @@
       <c r="E84" s="10"/>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="12"/>
       <c r="J84" s="10"/>
       <c r="K84" s="10"/>
       <c r="L84" s="10"/>
       <c r="M84" s="10"/>
       <c r="N84" s="10"/>
       <c r="O84" s="10"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P84" s="10"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -1932,16 +2021,17 @@
       <c r="E85" s="10"/>
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="12"/>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
       <c r="L85" s="10"/>
       <c r="M85" s="10"/>
       <c r="N85" s="10"/>
       <c r="O85" s="10"/>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P85" s="10"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -1949,16 +2039,17 @@
       <c r="E86" s="10"/>
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
-      <c r="H86" s="12"/>
-      <c r="I86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="10"/>
       <c r="K86" s="10"/>
       <c r="L86" s="10"/>
       <c r="M86" s="10"/>
       <c r="N86" s="10"/>
       <c r="O86" s="10"/>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P86" s="10"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
@@ -1966,16 +2057,17 @@
       <c r="E87" s="10"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
-      <c r="H87" s="12"/>
-      <c r="I87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="12"/>
       <c r="J87" s="10"/>
       <c r="K87" s="10"/>
       <c r="L87" s="10"/>
       <c r="M87" s="10"/>
       <c r="N87" s="10"/>
       <c r="O87" s="10"/>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P87" s="10"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -1983,16 +2075,17 @@
       <c r="E88" s="10"/>
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
-      <c r="H88" s="12"/>
-      <c r="I88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="12"/>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
       <c r="L88" s="10"/>
       <c r="M88" s="10"/>
       <c r="N88" s="10"/>
       <c r="O88" s="10"/>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P88" s="10"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -2000,16 +2093,17 @@
       <c r="E89" s="10"/>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
-      <c r="H89" s="12"/>
-      <c r="I89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="12"/>
       <c r="J89" s="10"/>
       <c r="K89" s="10"/>
       <c r="L89" s="10"/>
       <c r="M89" s="10"/>
       <c r="N89" s="10"/>
       <c r="O89" s="10"/>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P89" s="10"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -2017,16 +2111,17 @@
       <c r="E90" s="10"/>
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="12"/>
       <c r="J90" s="10"/>
       <c r="K90" s="10"/>
       <c r="L90" s="10"/>
       <c r="M90" s="10"/>
       <c r="N90" s="10"/>
       <c r="O90" s="10"/>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P90" s="10"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -2034,16 +2129,17 @@
       <c r="E91" s="10"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
-      <c r="H91" s="12"/>
-      <c r="I91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="12"/>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
       <c r="O91" s="10"/>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P91" s="10"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -2051,16 +2147,17 @@
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
-      <c r="H92" s="12"/>
-      <c r="I92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="12"/>
       <c r="J92" s="10"/>
       <c r="K92" s="10"/>
       <c r="L92" s="10"/>
       <c r="M92" s="10"/>
       <c r="N92" s="10"/>
       <c r="O92" s="10"/>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P92" s="10"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
@@ -2068,16 +2165,17 @@
       <c r="E93" s="10"/>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
-      <c r="H93" s="12"/>
-      <c r="I93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="12"/>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
       <c r="L93" s="10"/>
       <c r="M93" s="10"/>
       <c r="N93" s="10"/>
       <c r="O93" s="10"/>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P93" s="10"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -2085,16 +2183,17 @@
       <c r="E94" s="10"/>
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
-      <c r="H94" s="12"/>
-      <c r="I94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="12"/>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
       <c r="L94" s="10"/>
       <c r="M94" s="10"/>
       <c r="N94" s="10"/>
       <c r="O94" s="10"/>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P94" s="10"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
@@ -2102,16 +2201,17 @@
       <c r="E95" s="10"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
-      <c r="H95" s="12"/>
-      <c r="I95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="12"/>
       <c r="J95" s="10"/>
       <c r="K95" s="10"/>
       <c r="L95" s="10"/>
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
       <c r="O95" s="10"/>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P95" s="10"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -2119,16 +2219,17 @@
       <c r="E96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
-      <c r="H96" s="12"/>
-      <c r="I96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="12"/>
       <c r="J96" s="10"/>
       <c r="K96" s="10"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
       <c r="O96" s="10"/>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P96" s="10"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -2136,16 +2237,17 @@
       <c r="E97" s="10"/>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
-      <c r="H97" s="12"/>
-      <c r="I97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="12"/>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
       <c r="L97" s="10"/>
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
       <c r="O97" s="10"/>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P97" s="10"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -2153,16 +2255,17 @@
       <c r="E98" s="10"/>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
-      <c r="H98" s="12"/>
-      <c r="I98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="12"/>
       <c r="J98" s="10"/>
       <c r="K98" s="10"/>
       <c r="L98" s="10"/>
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
       <c r="O98" s="10"/>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P98" s="10"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -2170,16 +2273,17 @@
       <c r="E99" s="10"/>
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
-      <c r="H99" s="12"/>
-      <c r="I99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="12"/>
       <c r="J99" s="10"/>
       <c r="K99" s="10"/>
       <c r="L99" s="10"/>
       <c r="M99" s="10"/>
       <c r="N99" s="10"/>
       <c r="O99" s="10"/>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P99" s="10"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
@@ -2187,18 +2291,19 @@
       <c r="E100" s="10"/>
       <c r="F100" s="10"/>
       <c r="G100" s="10"/>
-      <c r="H100" s="12"/>
-      <c r="I100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="12"/>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
       <c r="L100" s="10"/>
       <c r="M100" s="10"/>
       <c r="N100" s="10"/>
       <c r="O100" s="10"/>
+      <c r="P100" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>